<commit_message>
Quick save checkpoint, in order to ensure branch exists in remote repo and before I start making significant changes to any module, data-file, notes, etc. (2024-05-31)
</commit_message>
<xml_diff>
--- a/files/data/example_grammar_parse_table_wb.xlsx
+++ b/files/data/example_grammar_parse_table_wb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickey/Desktop/Python/custom_packages/pyparse/files/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542A5722-11A2-DC4D-86DF-F05718C6093D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85473088-6BAE-A14A-9FCA-932657ACDC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{6BA989DE-F1A5-6E45-9F60-9D6D378D0973}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>STATE</t>
   </si>
@@ -87,13 +87,58 @@
   </si>
   <si>
     <t>ACCEPT (input accepted; parsing completed)</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>I#</t>
+  </si>
+  <si>
+    <t>ITEM SET/STATE #</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>I4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,17 +160,8 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,8 +174,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -188,42 +230,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -241,19 +257,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -570,101 +583,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C9148C-D6EF-0C4E-A505-2717DA2C2704}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
     <col min="12" max="12" width="38.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="8">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0</v>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K6" s="5" t="s">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K7" s="9" t="s">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K8" s="9" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="K8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K9" s="9" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="8" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="K10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="K11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Save checkpoint; updated the 'files/data/example_grammar_parse_table_wb.xlsx' parse table excel workbook (which, once complete and is accurate for desired example grammars, should be switched over to being of a '.csv' file format, so that the parse table contents can be read into memory, in a more system agnostic way, to be used for parsing during app/program's runtime (2024-04-31)
</commit_message>
<xml_diff>
--- a/files/data/example_grammar_parse_table_wb.xlsx
+++ b/files/data/example_grammar_parse_table_wb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickey/Desktop/Python/custom_packages/pyparse/files/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85473088-6BAE-A14A-9FCA-932657ACDC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AB21FA-1215-BC44-8858-C24B2D6AE30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{6BA989DE-F1A5-6E45-9F60-9D6D378D0973}"/>
+    <workbookView xWindow="7720" yWindow="2160" windowWidth="27640" windowHeight="16940" xr2:uid="{6BA989DE-F1A5-6E45-9F60-9D6D378D0973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>STATE</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>I4</t>
+  </si>
+  <si>
+    <t>TERMINALS</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
 </sst>
 </file>
@@ -234,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,6 +283,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +604,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -612,6 +630,10 @@
         <v>2</v>
       </c>
       <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -636,6 +658,7 @@
       <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -662,6 +685,9 @@
       <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -688,6 +714,9 @@
       <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -714,6 +743,9 @@
       <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -740,6 +772,9 @@
       <c r="H6" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>8</v>
       </c>
@@ -749,11 +784,30 @@
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
@@ -762,11 +816,33 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="K8" s="7" t="s">
         <v>10</v>
       </c>
@@ -996,9 +1072,10 @@
       <c r="H37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="B1:F1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Save checkpoint; saving draft designs so that I can pick back up where I left off (without the worry that I've deleted the work) (2024-06-01)
</commit_message>
<xml_diff>
--- a/files/data/example_grammar_parse_table_wb.xlsx
+++ b/files/data/example_grammar_parse_table_wb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickey/Desktop/Python/custom_packages/pyparse/files/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AB21FA-1215-BC44-8858-C24B2D6AE30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D4A47B-3687-5241-B263-42EED5E94D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="2160" windowWidth="27640" windowHeight="16940" xr2:uid="{6BA989DE-F1A5-6E45-9F60-9D6D378D0973}"/>
+    <workbookView xWindow="8440" yWindow="2900" windowWidth="25140" windowHeight="16140" xr2:uid="{6BA989DE-F1A5-6E45-9F60-9D6D378D0973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>STATE</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>R4</t>
+  </si>
+  <si>
+    <t>I6</t>
   </si>
 </sst>
 </file>
@@ -257,35 +260,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,9 +308,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,7 +348,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +454,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -593,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,49 +619,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="12"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="8">
+      <c r="A2" s="12"/>
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -775,10 +778,10 @@
       <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -808,10 +811,10 @@
       <c r="I7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -843,23 +846,26 @@
       <c r="I8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -869,10 +875,10 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="K10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="K10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -882,10 +888,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>